<commit_message>
Updated to AIDRES 2.0 data, chlorine data added, data of UK, CH and NO updated, sectors and processes missing in AIDRES added based on JRC-IDEES
</commit_message>
<xml_diff>
--- a/input_data/eurochlor_data/chlorine_data_2018.xlsx
+++ b/input_data/eurochlor_data/chlorine_data_2018.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vitoresearch-my.sharepoint.com/personal/partha_das_vito_be/Documents/Partha/work/times_veda/mopo/data_analysis_r/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vitoresearch-my.sharepoint.com/personal/hans_vandeput_vito_be/Documents/Mopo/mopo_repo/input_data/eurochlor_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="326" documentId="11_20D952506D2B4EF4CA4F014DB3EDCD69FA205DF7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{042A2AD2-1E7D-4B7C-B536-BF7B8D5445F8}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3005,7 +3005,7 @@
   <dimension ref="A1:M67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>